<commit_message>
Working version of 1D+1D+1D with magnetic field mapping
</commit_message>
<xml_diff>
--- a/source/APDL/Calculations.xlsx
+++ b/source/APDL/Calculations.xlsx
@@ -327,10 +327,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +614,7 @@
   <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,11 +857,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1029,11 +1029,11 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -1114,7 +1114,7 @@
         <v>3</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:G26" si="1">G23+$C$5</f>
+        <f t="shared" ref="G24:G25" si="1">G23+$C$5</f>
         <v>11.032000000000002</v>
       </c>
       <c r="H24">
@@ -1212,14 +1212,14 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <f>SUM(H22:H27)</f>
         <v>20741.622101924997</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit working 3D Mapping module
</commit_message>
<xml_diff>
--- a/source/APDL/Calculations.xlsx
+++ b/source/APDL/Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="931"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="931" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Deposition" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="102">
   <si>
     <t>strand_diameter</t>
   </si>
@@ -718,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="H22">
         <f>$C$28*(2*$C$21+2*$C$22+PI()*G22^2)</f>
-        <v>6715.3099547008569</v>
+        <v>10744.495927521371</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="H23">
         <f>$C$28*(2*$C$21+2*$C$22+PI()*G23^2)</f>
-        <v>6999.7148975863856</v>
+        <v>11199.543836138217</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="H24">
         <f t="shared" ref="H24:H25" si="0">$C$28*(2*$C$21+2*$C$22+PI()*G24^2)</f>
-        <v>7311.9380465168479</v>
+        <v>11699.100874426957</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
-        <v>7651.9794014922436</v>
+        <v>12243.167042387589</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>67</v>
       </c>
       <c r="C26">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -1647,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
@@ -1658,7 +1658,7 @@
         <v>68</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
         <v>3</v>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C30" s="6">
         <f>SUM(H22:H27)</f>
-        <v>28678.942300296334</v>
+        <v>45886.307680474136</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>1</v>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="C31">
         <f>C30*(C6-C4)</f>
-        <v>14357.708087699972</v>
+        <v>22972.332940319953</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -1704,8 +1704,8 @@
         <v>12</v>
       </c>
       <c r="C32">
-        <f>(2*C24+2*C25+4*C26)</f>
-        <v>680</v>
+        <f>(2*C24+2*C25)</f>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -1713,8 +1713,8 @@
         <v>75</v>
       </c>
       <c r="C33">
-        <f>(C28-1)*(C32+1)*C29</f>
-        <v>10896</v>
+        <f>(C32+1)*(C28-1)*C29</f>
+        <v>14588</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="C34">
         <f>(C29-1)*(C32+1)*C28</f>
-        <v>10215</v>
+        <v>12504</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C35">
         <f>SUM(C33:C34)</f>
-        <v>21111</v>
+        <v>27092</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="C36">
         <f>C31/C35</f>
-        <v>0.68010554155179626</v>
+        <v>0.84793787613760352</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="C38">
         <f>C36/C37</f>
-        <v>0.72274765308373679</v>
+        <v>0.90110295019936615</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
@@ -1776,10 +1776,10 @@
       </c>
       <c r="C39" s="1">
         <f>C38*0.000001</f>
-        <v>7.2274765308373677E-7</v>
+        <v>9.0110295019936609E-7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1794,8 +1794,8 @@
         <v>70</v>
       </c>
       <c r="C43">
-        <f>(C28*C27)*(2*C21+2*C22)</f>
-        <v>21600.799999999999</v>
+        <f>(C27)*(2*C21+2*C22)</f>
+        <v>34561.279999999999</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="C44">
         <f>C43*(C6-C4)</f>
-        <v>10814.135947321354</v>
+        <v>17302.617515714166</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="C46">
         <f>(C28-1)*(C45+1)*C29</f>
-        <v>8336</v>
+        <v>14588</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="C47">
         <f>(C29-1)*(C45+1)*C28</f>
-        <v>7815</v>
+        <v>12504</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1849,27 +1849,55 @@
       </c>
       <c r="C48">
         <f>SUM(C46:C47)</f>
-        <v>16151</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+        <v>27092</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f>C44/C48</f>
+        <v>0.63866150582142944</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <f>C37</f>
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f>C49/C50</f>
+        <v>0.67870510714285814</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>79</v>
+      </c>
+      <c r="C52" s="1">
+        <f>C51*0.000001</f>
+        <v>6.7870510714285809E-7</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 3D Mapping, comments added in each class
</commit_message>
<xml_diff>
--- a/source/APDL/Calculations.xlsx
+++ b/source/APDL/Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="931" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="931" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Heat Deposition" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="114">
   <si>
     <t>strand_diameter</t>
   </si>
@@ -333,6 +333,42 @@
   </si>
   <si>
     <t>rounded part negligible</t>
+  </si>
+  <si>
+    <t>case 1D+1D+1D effective length and area</t>
+  </si>
+  <si>
+    <t>effective_conduction_side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winding_length </t>
+  </si>
+  <si>
+    <t>no_insulation_elements</t>
+  </si>
+  <si>
+    <t>total_insulation_area</t>
+  </si>
+  <si>
+    <t>average_insulation_perimeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm </t>
+  </si>
+  <si>
+    <t>insulation_thickness</t>
+  </si>
+  <si>
+    <t>effective_insulation_area</t>
+  </si>
+  <si>
+    <t>insulation_volume</t>
+  </si>
+  <si>
+    <t>element_insulation_area_constant (method1)</t>
+  </si>
+  <si>
+    <t>element_insulation_area_constant (method2)</t>
   </si>
 </sst>
 </file>
@@ -372,15 +408,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -388,20 +430,130 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1121,7 +1273,7 @@
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1327,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H52"/>
+  <dimension ref="B1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,568 +1495,825 @@
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>0.7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <f xml:space="preserve"> C3^2/4*PI()</f>
         <v>0.38484510006474959</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>0.94099999999999995</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <f>C5^2</f>
         <v>0.88548099999999985</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="11">
         <v>1000</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <f>(C6-C4)*C7</f>
         <v>500.63589993525028</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <f>C9*C8</f>
         <v>2503.1794996762515</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="9" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+    </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="11">
         <v>100</v>
       </c>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
         <f>C12+1</f>
         <v>101</v>
       </c>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <f>C13*(C9-1)</f>
         <v>404</v>
       </c>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="8">
         <f>C10/C14</f>
         <v>6.195988860584781</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="8">
         <v>0.94099999999999995</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="8">
         <f>C15/C16</f>
         <v>6.5844727530125198</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="14">
         <f>C17*0.000001</f>
         <v>6.5844727530125191E-6</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="15" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="8">
         <v>413.21</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="8">
         <v>126.81</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F22">
+      <c r="E22" s="8"/>
+      <c r="F22" s="8">
         <v>1</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="8">
         <f>C23</f>
         <v>9.15</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="9">
         <f>$C$28*(2*$C$21+2*$C$22+PI()*G22^2)</f>
-        <v>10744.495927521371</v>
+        <v>6715.3099547008569</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <f>(9+0.15)</f>
         <v>9.15</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F23">
+      <c r="E23" s="8"/>
+      <c r="F23" s="8">
         <v>2</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="8">
         <f>G22+$C$5</f>
         <v>10.091000000000001</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="9">
         <f>$C$28*(2*$C$21+2*$C$22+PI()*G23^2)</f>
-        <v>11199.543836138217</v>
+        <v>6999.7148975863856</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C24">
-        <v>200</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="8">
+        <v>100</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F24">
+      <c r="E24" s="8"/>
+      <c r="F24" s="8">
         <v>3</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="8">
         <f>G23+$C$5</f>
         <v>11.032000000000002</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="9">
         <f t="shared" ref="H24:H25" si="0">$C$28*(2*$C$21+2*$C$22+PI()*G24^2)</f>
-        <v>11699.100874426957</v>
+        <v>7311.9380465168479</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C25">
-        <v>60</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="8">
+        <v>30</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F25">
+      <c r="E25" s="8"/>
+      <c r="F25" s="8">
         <v>4</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="8">
         <f>G24+$C$5</f>
         <v>11.973000000000003</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="9">
         <f t="shared" si="0"/>
-        <v>12243.167042387589</v>
+        <v>7651.9794014922436</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="8">
+        <v>5</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C27" s="8">
+        <v>45</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="8">
+        <v>5</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28">
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="8">
+        <v>9</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="17">
+        <f>SUM(H22:H27)</f>
+        <v>28678.942300296334</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="8">
+        <f>C30*(C6-C4)</f>
+        <v>14357.708087699972</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="8">
+        <f>(2*C24+2*C25)</f>
+        <v>260</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="8">
+        <f>(C32+1)*(C28-1)*C29</f>
+        <v>9396</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="8">
+        <f>(C29-1)*(C32+1)*C28</f>
+        <v>10440</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="8">
+        <f>SUM(C33:C34)</f>
+        <v>19836</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="8">
+        <f>C31/C35</f>
+        <v>0.72382073440713712</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="8">
+        <f>C36/C37</f>
+        <v>0.76920375601183544</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="14">
+        <f>C38*0.000001</f>
+        <v>7.6920375601183543E-7</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19"/>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="30"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="6">
-        <f>SUM(H22:H27)</f>
-        <v>45886.307680474136</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="C43" s="8">
+        <f>(C27)*(2*C21+2*C22)</f>
+        <v>48601.799999999996</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="E43" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="21"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C31">
-        <f>C30*(C6-C4)</f>
-        <v>22972.332940319953</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C44" s="8">
+        <f>C43*(C6-C4)</f>
+        <v>24331.805881473043</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C32">
-        <f>(2*C24+2*C25)</f>
-        <v>520</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="C45" s="8">
+        <f>2*C24+2*C25</f>
+        <v>260</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C33">
-        <f>(C32+1)*(C28-1)*C29</f>
-        <v>14588</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="C46" s="8">
+        <f>(C28-1)*(C45+1)*C29</f>
+        <v>9396</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C34">
-        <f>(C29-1)*(C32+1)*C28</f>
-        <v>12504</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="C47" s="8">
+        <f>(C29-1)*(C45+1)*C28</f>
+        <v>10440</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C35">
-        <f>SUM(C33:C34)</f>
-        <v>27092</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="C48" s="8">
+        <f>SUM(C46:C47)</f>
+        <v>19836</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C36">
-        <f>C31/C35</f>
-        <v>0.84793787613760352</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C49" s="8">
+        <f>C44/C48</f>
+        <v>1.226648814351333</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="E49" s="8"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C37">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38">
-        <f>C36/C37</f>
-        <v>0.90110295019936615</v>
-      </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="1">
-        <f>C38*0.000001</f>
-        <v>9.0110295019936609E-7</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43">
-        <f>(C27)*(2*C21+2*C22)</f>
-        <v>34561.279999999999</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44">
-        <f>C43*(C6-C4)</f>
-        <v>17302.617515714166</v>
-      </c>
-      <c r="D44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45">
-        <f>2*C24+2*C25</f>
-        <v>520</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46">
-        <f>(C28-1)*(C45+1)*C29</f>
-        <v>14588</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47">
-        <f>(C29-1)*(C45+1)*C28</f>
-        <v>12504</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48">
-        <f>SUM(C46:C47)</f>
-        <v>27092</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49">
-        <f>C44/C48</f>
-        <v>0.63866150582142944</v>
-      </c>
-      <c r="D49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50">
+      <c r="C50" s="8">
         <f>C37</f>
         <v>0.94099999999999995</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="E50" s="8"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="8">
         <f>C49/C50</f>
-        <v>0.67870510714285814</v>
-      </c>
-      <c r="D51" t="s">
+        <v>1.3035587825200139</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
+      <c r="E51" s="8"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="14">
         <f>C51*0.000001</f>
-        <v>6.7870510714285809E-7</v>
-      </c>
-      <c r="D52" s="1" t="s">
+        <v>1.3035587825200137E-6</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>33</v>
       </c>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19"/>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="30"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="8">
+        <f>C6-C4</f>
+        <v>0.50063589993525026</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="8">
+        <f>(C3*PI()+4*C5)/2</f>
+        <v>2.9815574287564273</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="8">
+        <f>C56/4</f>
+        <v>0.74538935718910682</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="8">
+        <f>C55/C56</f>
+        <v>0.16791086936871769</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="8">
+        <f>C55/4</f>
+        <v>0.12515897498381257</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="8">
+        <f>(2*C22+2*C21)</f>
+        <v>1080.04</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="8">
+        <f>2*(1+C24)+2*(1+C25)</f>
+        <v>264</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="8">
+        <f>C60*C59</f>
+        <v>135.17669934151692</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="11">
+        <f>(C62/C58)/C61*0.001^2</f>
+        <v>3.0494330353731926E-6</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="14">
+        <f>C57*C60/C61*0.001^2</f>
+        <v>3.0494330353731922E-6</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="18"/>
+      <c r="F64" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>